<commit_message>
Indicatori Matteo & Noemi
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>Action</t>
   </si>
@@ -156,16 +156,67 @@
     <t>INDICATOR_1</t>
   </si>
   <si>
-    <t>INDICATOR_2</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
+    <t>updateAnalyticaltable</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>updateAnalyticaltable_BE</t>
+    <t>INDICATOR_3</t>
+  </si>
+  <si>
+    <t>INDICATOR_20</t>
+  </si>
+  <si>
+    <t>INDICATOR_55</t>
+  </si>
+  <si>
+    <t>INDICATOR_210</t>
+  </si>
+  <si>
+    <t>INDICATOR_218</t>
+  </si>
+  <si>
+    <t>INDICATOR_16</t>
+  </si>
+  <si>
+    <t>INDICATOR_50</t>
+  </si>
+  <si>
+    <t>INDICATOR_197</t>
+  </si>
+  <si>
+    <t>INDICATOR_213</t>
+  </si>
+  <si>
+    <t>INDICATOR_217</t>
+  </si>
+  <si>
+    <t>INDICATOR_14</t>
+  </si>
+  <si>
+    <t>INDICATOR_49</t>
+  </si>
+  <si>
+    <t>INDICATOR_193</t>
+  </si>
+  <si>
+    <t>INDICATOR_212</t>
+  </si>
+  <si>
+    <t>INDICATOR_216</t>
+  </si>
+  <si>
+    <t>INDICATOR_44</t>
+  </si>
+  <si>
+    <t>INDICATOR_58</t>
+  </si>
+  <si>
+    <t>INDICATOR_211</t>
   </si>
 </sst>
 </file>
@@ -244,7 +295,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -757,10 +808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -805,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -815,11 +866,11 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -830,10 +881,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -847,7 +898,245 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicatori BIB complessità 2 e 3 Matteo
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
   <si>
     <t>Action</t>
   </si>
@@ -216,7 +216,67 @@
     <t>INDICATOR_58</t>
   </si>
   <si>
-    <t>INDICATOR_211</t>
+    <t xml:space="preserve">INDICATOR_211 </t>
+  </si>
+  <si>
+    <t>INDICATOR_35</t>
+  </si>
+  <si>
+    <t>INDICATOR_56</t>
+  </si>
+  <si>
+    <t>INDICATOR_60</t>
+  </si>
+  <si>
+    <t>INDICATOR_66</t>
+  </si>
+  <si>
+    <t>INDICATOR_70</t>
+  </si>
+  <si>
+    <t>INDICATOR_76</t>
+  </si>
+  <si>
+    <t>INDICATOR_80</t>
+  </si>
+  <si>
+    <t>INDICATOR_84</t>
+  </si>
+  <si>
+    <t>INDICATOR_88</t>
+  </si>
+  <si>
+    <t>INDICATOR_92</t>
+  </si>
+  <si>
+    <t>INDICATOR_96</t>
+  </si>
+  <si>
+    <t>INDICATOR_100</t>
+  </si>
+  <si>
+    <t>INDICATOR_105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_113 </t>
+  </si>
+  <si>
+    <t>INDICATOR_118</t>
+  </si>
+  <si>
+    <t>INDICATOR_124</t>
+  </si>
+  <si>
+    <t>INDICATOR_128</t>
+  </si>
+  <si>
+    <t>INDICATOR_132</t>
+  </si>
+  <si>
+    <t>INDICATOR_173</t>
+  </si>
+  <si>
+    <t>INDICATOR_186</t>
   </si>
 </sst>
 </file>
@@ -295,7 +355,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -909,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -923,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -937,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -951,7 +1011,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -965,7 +1025,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -993,7 +1053,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -1007,7 +1067,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1021,7 +1081,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1035,7 +1095,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>17</v>
@@ -1049,7 +1109,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1063,7 +1123,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1091,7 +1151,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>17</v>
@@ -1105,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1119,7 +1179,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1133,9 +1193,289 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1297,18 +1637,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1328,6 +1668,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1340,12 +1688,4 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Indicatori BIB complessità 2 Matteo, Noemi e Gian Carlo
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="96">
   <si>
     <t>Action</t>
   </si>
@@ -216,9 +216,6 @@
     <t>INDICATOR_58</t>
   </si>
   <si>
-    <t xml:space="preserve">INDICATOR_211 </t>
-  </si>
-  <si>
     <t>INDICATOR_35</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>INDICATOR_105</t>
   </si>
   <si>
-    <t xml:space="preserve">INDICATOR_113 </t>
-  </si>
-  <si>
     <t>INDICATOR_118</t>
   </si>
   <si>
@@ -277,6 +271,126 @@
   </si>
   <si>
     <t>INDICATOR_186</t>
+  </si>
+  <si>
+    <t>INDICATOR_211</t>
+  </si>
+  <si>
+    <t>INDICATOR_2</t>
+  </si>
+  <si>
+    <t>INDICATOR_7</t>
+  </si>
+  <si>
+    <t>INDICATOR_9</t>
+  </si>
+  <si>
+    <t>INDICATOR_34</t>
+  </si>
+  <si>
+    <t>INDICATOR_48</t>
+  </si>
+  <si>
+    <t>INDICATOR_51</t>
+  </si>
+  <si>
+    <t>INDICATOR_64</t>
+  </si>
+  <si>
+    <t>INDICATOR_69</t>
+  </si>
+  <si>
+    <t>INDICATOR_74</t>
+  </si>
+  <si>
+    <t>INDICATOR_75</t>
+  </si>
+  <si>
+    <t>INDICATOR_78</t>
+  </si>
+  <si>
+    <t>INDICATOR_79</t>
+  </si>
+  <si>
+    <t>INDICATOR_82</t>
+  </si>
+  <si>
+    <t>INDICATOR_83</t>
+  </si>
+  <si>
+    <t>INDICATOR_86</t>
+  </si>
+  <si>
+    <t>INDICATOR_87</t>
+  </si>
+  <si>
+    <t>INDICATOR_90</t>
+  </si>
+  <si>
+    <t>INDICATOR_91</t>
+  </si>
+  <si>
+    <t>INDICATOR_94</t>
+  </si>
+  <si>
+    <t>INDICATOR_95</t>
+  </si>
+  <si>
+    <t>INDICATOR_97</t>
+  </si>
+  <si>
+    <t>INDICATOR_99</t>
+  </si>
+  <si>
+    <t>INDICATOR_103</t>
+  </si>
+  <si>
+    <t>INDICATOR_104</t>
+  </si>
+  <si>
+    <t>INDICATOR_107</t>
+  </si>
+  <si>
+    <t>INDICATOR_108</t>
+  </si>
+  <si>
+    <t>INDICATOR_111</t>
+  </si>
+  <si>
+    <t>INDICATOR_112</t>
+  </si>
+  <si>
+    <t>INDICATOR_113</t>
+  </si>
+  <si>
+    <t>INDICATOR_115</t>
+  </si>
+  <si>
+    <t>INDICATOR_116</t>
+  </si>
+  <si>
+    <t>INDICATOR_120</t>
+  </si>
+  <si>
+    <t>INDICATOR_121</t>
+  </si>
+  <si>
+    <t>INDICATOR_126</t>
+  </si>
+  <si>
+    <t>INDICATOR_127</t>
+  </si>
+  <si>
+    <t>INDICATOR_130</t>
+  </si>
+  <si>
+    <t>INDICATOR_131</t>
+  </si>
+  <si>
+    <t>INDICATOR_182</t>
+  </si>
+  <si>
+    <t>INDICATOR_205</t>
   </si>
 </sst>
 </file>
@@ -295,22 +409,26 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -355,7 +473,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -868,11 +986,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1123,7 +1239,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1207,7 +1323,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1221,7 +1337,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1235,7 +1351,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1249,7 +1365,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1263,7 +1379,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1277,7 +1393,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1291,7 +1407,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1305,7 +1421,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1319,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1333,7 +1449,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1347,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1361,7 +1477,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1375,7 +1491,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1389,7 +1505,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1403,7 +1519,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1417,7 +1533,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1431,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1445,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1459,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1473,9 +1589,541 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1523,6 +2171,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1636,22 +2299,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1665,27 +2336,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Indicatori BIB complessità 2 Roberto
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.pandino\Desktop\GIT_Tortoise\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="115">
   <si>
     <t>Action</t>
   </si>
@@ -391,6 +391,63 @@
   </si>
   <si>
     <t>INDICATOR_205</t>
+  </si>
+  <si>
+    <t>INDICATOR_40</t>
+  </si>
+  <si>
+    <t>INDICATOR_57</t>
+  </si>
+  <si>
+    <t>INDICATOR_71</t>
+  </si>
+  <si>
+    <t>INDICATOR_77</t>
+  </si>
+  <si>
+    <t>INDICATOR_81</t>
+  </si>
+  <si>
+    <t>INDICATOR_85</t>
+  </si>
+  <si>
+    <t>INDICATOR_89</t>
+  </si>
+  <si>
+    <t>INDICATOR_93</t>
+  </si>
+  <si>
+    <t>INDICATOR_98</t>
+  </si>
+  <si>
+    <t>INDICATOR_102</t>
+  </si>
+  <si>
+    <t>INDICATOR_106</t>
+  </si>
+  <si>
+    <t>INDICATOR_110</t>
+  </si>
+  <si>
+    <t>INDICATOR_114</t>
+  </si>
+  <si>
+    <t>INDICATOR_119</t>
+  </si>
+  <si>
+    <t>INDICATOR_125</t>
+  </si>
+  <si>
+    <t>INDICATOR_129</t>
+  </si>
+  <si>
+    <t>INDICATOR_133</t>
+  </si>
+  <si>
+    <t>INDICATOR_181</t>
+  </si>
+  <si>
+    <t>INDICATOR_201</t>
   </si>
 </sst>
 </file>
@@ -473,7 +530,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -986,9 +1043,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80:E99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1393,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1407,7 +1466,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1421,7 +1480,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1435,7 +1494,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1449,7 +1508,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1463,7 +1522,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1477,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1491,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1505,7 +1564,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1519,7 +1578,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1533,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1547,7 +1606,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1561,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1575,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1589,7 +1648,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1603,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1617,7 +1676,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1631,7 +1690,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1645,7 +1704,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1659,7 +1718,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1673,7 +1732,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1687,7 +1746,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1701,7 +1760,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1715,7 +1774,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1729,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1743,7 +1802,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1757,7 +1816,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1771,7 +1830,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1785,7 +1844,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1799,7 +1858,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1813,7 +1872,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1827,7 +1886,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1841,7 +1900,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1855,7 +1914,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1869,7 +1928,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1883,7 +1942,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1897,7 +1956,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -1911,7 +1970,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -1925,7 +1984,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -1939,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -1953,7 +2012,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -1967,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -1981,7 +2040,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -1995,7 +2054,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2009,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2023,7 +2082,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2037,7 +2096,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2051,7 +2110,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2065,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2079,7 +2138,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2093,7 +2152,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2107,7 +2166,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2121,9 +2180,275 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2171,21 +2496,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2299,17 +2609,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2323,17 +2649,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunti indicatori BIB livello 3
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.pandino\Desktop\GIT_Tortoise\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="126">
   <si>
     <t>Action</t>
   </si>
@@ -448,6 +448,39 @@
   </si>
   <si>
     <t>INDICATOR_201</t>
+  </si>
+  <si>
+    <t>INDICATOR_8</t>
+  </si>
+  <si>
+    <t>INDICATOR_13</t>
+  </si>
+  <si>
+    <t>INDICATOR_59</t>
+  </si>
+  <si>
+    <t>INDICATOR_61</t>
+  </si>
+  <si>
+    <t>INDICATOR_62</t>
+  </si>
+  <si>
+    <t>INDICATOR_63</t>
+  </si>
+  <si>
+    <t>INDICATOR_67</t>
+  </si>
+  <si>
+    <t>INDICATOR_68</t>
+  </si>
+  <si>
+    <t>INDICATOR_172</t>
+  </si>
+  <si>
+    <t>INDICATOR_187</t>
+  </si>
+  <si>
+    <t>INDICATOR_188</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80:E99"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2449,6 +2482,160 @@
         <v>95</v>
       </c>
       <c r="E99" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2496,6 +2683,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2609,22 +2811,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2638,27 +2848,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Indicatori corretti (11, 34, 44)
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noemi.careddu\Desktop\Noemi\EW_BIB\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="127">
   <si>
     <t>Action</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>INDICATOR_188</t>
+  </si>
+  <si>
+    <t>INDICATOR_11</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1180,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -1191,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -1205,7 +1208,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -1219,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -1233,7 +1236,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -1247,7 +1250,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1261,7 +1264,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -1275,7 +1278,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1289,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1303,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>17</v>
@@ -1317,7 +1320,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1331,7 +1334,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1345,7 +1348,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -1359,7 +1362,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>17</v>
@@ -1373,7 +1376,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1387,7 +1390,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1401,7 +1404,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1414,8 +1417,8 @@
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>57</v>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1429,7 +1432,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1443,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1457,7 +1460,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1471,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1485,7 +1488,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1499,7 +1502,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1513,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1527,7 +1530,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1541,7 +1544,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1555,7 +1558,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1569,7 +1572,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1583,7 +1586,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1597,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1611,7 +1614,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1625,7 +1628,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1639,7 +1642,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1653,7 +1656,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1667,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1681,7 +1684,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1695,7 +1698,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1709,7 +1712,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1723,7 +1726,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1737,7 +1740,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1751,7 +1754,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1765,7 +1768,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1779,7 +1782,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1793,7 +1796,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1807,7 +1810,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1821,7 +1824,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1835,7 +1838,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1849,7 +1852,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1863,7 +1866,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1877,7 +1880,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1891,7 +1894,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1905,7 +1908,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1919,7 +1922,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1933,7 +1936,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1947,7 +1950,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1961,7 +1964,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1975,7 +1978,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1989,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2003,7 +2006,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2017,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2031,7 +2034,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2045,7 +2048,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2059,7 +2062,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2073,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2087,7 +2090,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2101,7 +2104,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2115,7 +2118,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2129,7 +2132,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2143,7 +2146,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2157,7 +2160,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2171,7 +2174,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2185,7 +2188,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2199,7 +2202,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2213,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2227,7 +2230,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2241,7 +2244,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2255,7 +2258,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2269,7 +2272,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2283,7 +2286,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2297,7 +2300,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2311,7 +2314,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2325,7 +2328,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2339,7 +2342,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2353,7 +2356,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2367,7 +2370,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2381,7 +2384,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2395,7 +2398,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2409,7 +2412,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2423,7 +2426,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2437,7 +2440,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2451,7 +2454,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2465,7 +2468,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2479,7 +2482,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2492,8 +2495,8 @@
       <c r="B100" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>115</v>
+      <c r="C100" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2507,7 +2510,7 @@
         <v>13</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2521,7 +2524,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2535,7 +2538,7 @@
         <v>13</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2549,7 +2552,7 @@
         <v>13</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2563,7 +2566,7 @@
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2577,7 +2580,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2591,7 +2594,7 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2605,7 +2608,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2619,7 +2622,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2633,9 +2636,23 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2683,21 +2700,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2811,17 +2813,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2835,17 +2853,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Indicatori corretti ( 11, 51, 58, 59, 63, 69, 75, 79, 83, 87, 91, 95, 99, 104, 108, 112, 116, 121, 127, 131, 172, 211, 215)
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="128">
   <si>
     <t>Action</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>INDICATOR_11</t>
+  </si>
+  <si>
+    <t>INDICATOR_215</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1390,7 +1393,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1404,7 +1407,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1418,7 +1421,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1431,8 +1434,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>57</v>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1446,7 +1449,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1460,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1474,7 +1477,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1488,7 +1491,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1502,7 +1505,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1516,7 +1519,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1530,7 +1533,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1544,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1558,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1572,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1586,7 +1589,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1600,7 +1603,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1614,7 +1617,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1628,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1642,7 +1645,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1656,7 +1659,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1670,7 +1673,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1684,7 +1687,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1698,7 +1701,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1712,7 +1715,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1726,7 +1729,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1740,7 +1743,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1754,7 +1757,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1768,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1782,7 +1785,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1796,7 +1799,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1810,7 +1813,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1824,7 +1827,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1838,7 +1841,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1852,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1866,7 +1869,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1880,7 +1883,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1894,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1908,7 +1911,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1922,7 +1925,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1936,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1950,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1964,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1978,7 +1981,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1992,7 +1995,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2006,7 +2009,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2020,7 +2023,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2034,7 +2037,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2048,7 +2051,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2062,7 +2065,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2076,7 +2079,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2090,7 +2093,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2104,7 +2107,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2118,7 +2121,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2132,7 +2135,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2146,7 +2149,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2160,7 +2163,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2174,7 +2177,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2188,7 +2191,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2202,7 +2205,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2216,7 +2219,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2230,7 +2233,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2244,7 +2247,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2258,7 +2261,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2272,7 +2275,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2286,7 +2289,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2300,7 +2303,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2314,7 +2317,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2328,7 +2331,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2342,7 +2345,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2356,7 +2359,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2370,7 +2373,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2384,7 +2387,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2398,7 +2401,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2412,7 +2415,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2426,7 +2429,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2440,7 +2443,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2454,7 +2457,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2468,7 +2471,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2482,7 +2485,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2496,7 +2499,7 @@
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2509,8 +2512,8 @@
       <c r="B101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>115</v>
+      <c r="C101" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2524,7 +2527,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2538,7 +2541,7 @@
         <v>13</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2552,7 +2555,7 @@
         <v>13</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2566,7 +2569,7 @@
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2580,7 +2583,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2594,7 +2597,7 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2608,7 +2611,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2622,7 +2625,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2636,7 +2639,7 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>17</v>
@@ -2650,9 +2653,23 @@
         <v>13</v>
       </c>
       <c r="C111" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornamento formula Union_Indicators e file Excel LibFormula
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noemi.careddu\Desktop\Noemi\EW_BIB\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="129">
   <si>
     <t>Action</t>
   </si>
@@ -222,9 +222,6 @@
     <t>INDICATOR_56</t>
   </si>
   <si>
-    <t>INDICATOR_60</t>
-  </si>
-  <si>
     <t>INDICATOR_66</t>
   </si>
   <si>
@@ -453,33 +450,21 @@
     <t>INDICATOR_8</t>
   </si>
   <si>
-    <t>INDICATOR_13</t>
-  </si>
-  <si>
     <t>INDICATOR_59</t>
   </si>
   <si>
-    <t>INDICATOR_61</t>
-  </si>
-  <si>
     <t>INDICATOR_62</t>
   </si>
   <si>
     <t>INDICATOR_63</t>
   </si>
   <si>
-    <t>INDICATOR_67</t>
-  </si>
-  <si>
     <t>INDICATOR_68</t>
   </si>
   <si>
     <t>INDICATOR_172</t>
   </si>
   <si>
-    <t>INDICATOR_187</t>
-  </si>
-  <si>
     <t>INDICATOR_188</t>
   </si>
   <si>
@@ -487,6 +472,24 @@
   </si>
   <si>
     <t>INDICATOR_215</t>
+  </si>
+  <si>
+    <t>INDICATOR_109</t>
+  </si>
+  <si>
+    <t>INDICATOR_174</t>
+  </si>
+  <si>
+    <t>INDICATOR_175</t>
+  </si>
+  <si>
+    <t>INDICATOR_180</t>
+  </si>
+  <si>
+    <t>INDICATOR_183</t>
+  </si>
+  <si>
+    <t>INDICATOR_214</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1082,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112:E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1169,7 +1172,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
@@ -1183,7 +1186,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -1197,7 +1200,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -1211,7 +1214,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -1225,7 +1228,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -1239,7 +1242,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -1253,7 +1256,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1267,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -1281,7 +1284,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1295,7 +1298,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1309,7 +1312,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>17</v>
@@ -1323,7 +1326,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1337,7 +1340,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1351,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -1365,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>17</v>
@@ -1379,7 +1382,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1393,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1407,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1421,7 +1424,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1435,7 +1438,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1449,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1463,7 +1466,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1477,7 +1480,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1491,7 +1494,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1505,7 +1508,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1519,7 +1522,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1533,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1547,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1561,7 +1564,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1589,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1603,7 +1606,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1617,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1631,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1645,7 +1648,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1659,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1673,7 +1676,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1687,7 +1690,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1701,7 +1704,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1715,7 +1718,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1729,7 +1732,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1743,7 +1746,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1757,7 +1760,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1771,7 +1774,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1785,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1799,7 +1802,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1813,7 +1816,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1827,7 +1830,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1841,7 +1844,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1855,7 +1858,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1869,7 +1872,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1883,7 +1886,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1897,7 +1900,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1911,7 +1914,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1925,7 +1928,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1939,7 +1942,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1953,7 +1956,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1967,7 +1970,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1981,7 +1984,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1995,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2009,7 +2012,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2023,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2037,7 +2040,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2051,7 +2054,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2065,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2079,7 +2082,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2093,7 +2096,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2107,7 +2110,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2121,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2135,7 +2138,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2149,7 +2152,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2163,7 +2166,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2177,7 +2180,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2191,7 +2194,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2205,7 +2208,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2219,7 +2222,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2233,7 +2236,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2247,7 +2250,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2261,7 +2264,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2275,7 +2278,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2289,7 +2292,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2303,7 +2306,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2317,7 +2320,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2331,7 +2334,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2345,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2359,7 +2362,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2373,7 +2376,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2387,7 +2390,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2401,7 +2404,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2415,7 +2418,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2429,7 +2432,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2443,7 +2446,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2457,7 +2460,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2471,7 +2474,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2485,7 +2488,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2499,7 +2502,7 @@
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2513,7 +2516,7 @@
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2527,7 +2530,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2541,7 +2544,7 @@
         <v>13</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2555,7 +2558,7 @@
         <v>13</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2569,7 +2572,7 @@
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2583,7 +2586,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2597,7 +2600,7 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2611,7 +2614,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2625,7 +2628,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2639,7 +2642,7 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>17</v>
@@ -2653,7 +2656,7 @@
         <v>13</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>17</v>
@@ -2667,9 +2670,23 @@
         <v>13</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="E112" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2831,18 +2848,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2862,14 +2879,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2882,4 +2891,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornamento Indicatori BIB, Union e Lib_Formula
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meloni.luca\Desktop\ATS\EarlyWarning\estere\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="132">
   <si>
     <t>Action</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>INDICATOR_214</t>
+  </si>
+  <si>
+    <t>INDICATOR_187</t>
+  </si>
+  <si>
+    <t>INDICATOR_60</t>
+  </si>
+  <si>
+    <t>INDICATOR_61</t>
   </si>
 </sst>
 </file>
@@ -572,7 +581,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1085,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112:E113"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1476,11 +1485,11 @@
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>116</v>
+      <c r="B27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1490,11 +1499,11 @@
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>117</v>
+      <c r="B28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1508,7 +1517,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1522,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1536,7 +1545,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1550,7 +1559,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1564,7 +1573,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1578,7 +1587,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1592,7 +1601,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1606,7 +1615,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1620,7 +1629,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1634,7 +1643,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1648,7 +1657,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1662,7 +1671,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1676,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1690,7 +1699,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1704,7 +1713,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1718,7 +1727,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1732,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1746,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1760,7 +1769,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1774,7 +1783,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1788,7 +1797,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1802,7 +1811,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1816,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1830,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1844,7 +1853,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1858,7 +1867,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1872,7 +1881,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1886,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1900,7 +1909,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1914,7 +1923,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1928,7 +1937,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1942,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1956,7 +1965,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1970,7 +1979,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1984,7 +1993,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1998,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2012,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2026,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2040,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2054,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2068,7 +2077,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2082,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2096,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2110,7 +2119,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2124,7 +2133,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2138,7 +2147,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2152,7 +2161,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2166,7 +2175,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2180,7 +2189,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2194,7 +2203,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2208,7 +2217,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2222,7 +2231,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2236,7 +2245,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2250,7 +2259,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2264,7 +2273,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2278,7 +2287,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2292,7 +2301,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2306,7 +2315,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2320,7 +2329,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2334,7 +2343,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2348,7 +2357,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2362,7 +2371,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2376,7 +2385,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2390,7 +2399,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2404,7 +2413,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2418,7 +2427,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>125</v>
+        <v>53</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2432,7 +2441,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2446,7 +2455,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2460,7 +2469,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2474,7 +2483,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2488,7 +2497,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2502,7 +2511,7 @@
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2516,7 +2525,7 @@
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2526,11 +2535,11 @@
       <c r="A102" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2543,8 +2552,8 @@
       <c r="B103" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>113</v>
+      <c r="C103" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2557,8 +2566,8 @@
       <c r="B104" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>94</v>
+      <c r="C104" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2572,7 +2581,7 @@
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2586,7 +2595,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2600,7 +2609,7 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2614,7 +2623,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2628,7 +2637,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2642,7 +2651,7 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>17</v>
@@ -2656,7 +2665,7 @@
         <v>13</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>17</v>
@@ -2670,7 +2679,7 @@
         <v>13</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>17</v>
@@ -2680,13 +2689,55 @@
       <c r="A113" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E116" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2848,18 +2899,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2879,6 +2930,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2891,12 +2950,4 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunta indicatore 15 BIB
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="134">
   <si>
     <t>Action</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>ExternalInfo</t>
+  </si>
+  <si>
+    <t>INDICATOR_15</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C113" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2761,6 +2764,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2773,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2805,12 +2822,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2928,15 +2942,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2958,16 +2982,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modifica ndicatore 11, eliminazione degli indicatori 59, 118, 119, 120 e 121
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noemi.careddu\Desktop\Noemi\EW_BIB\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="133">
   <si>
     <t>Action</t>
   </si>
@@ -249,9 +249,6 @@
     <t>INDICATOR_105</t>
   </si>
   <si>
-    <t>INDICATOR_118</t>
-  </si>
-  <si>
     <t>INDICATOR_124</t>
   </si>
   <si>
@@ -363,12 +360,6 @@
     <t>INDICATOR_116</t>
   </si>
   <si>
-    <t>INDICATOR_120</t>
-  </si>
-  <si>
-    <t>INDICATOR_121</t>
-  </si>
-  <si>
     <t>INDICATOR_126</t>
   </si>
   <si>
@@ -426,9 +417,6 @@
     <t>INDICATOR_114</t>
   </si>
   <si>
-    <t>INDICATOR_119</t>
-  </si>
-  <si>
     <t>INDICATOR_125</t>
   </si>
   <si>
@@ -511,6 +499,9 @@
   </si>
   <si>
     <t>INDICATOR_11</t>
+  </si>
+  <si>
+    <t>Real</t>
   </si>
 </sst>
 </file>
@@ -1106,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1156,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -1193,7 +1184,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
@@ -1221,7 +1212,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -1235,7 +1226,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -1249,7 +1240,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -1263,10 +1254,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1277,7 +1268,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1305,7 +1296,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1347,7 +1338,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1375,7 +1366,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -1403,7 +1394,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1445,7 +1436,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1487,7 +1478,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1515,7 +1506,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1529,7 +1520,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1543,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1557,7 +1548,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1571,7 +1562,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1585,7 +1576,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1613,7 +1604,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1627,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1641,7 +1632,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1669,7 +1660,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1683,7 +1674,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1697,7 +1688,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1725,7 +1716,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1739,7 +1730,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1753,7 +1744,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1781,7 +1772,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1795,7 +1786,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1809,7 +1800,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1837,7 +1828,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1851,7 +1842,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1865,7 +1856,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1893,7 +1884,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1907,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1921,7 +1912,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1949,7 +1940,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1963,7 +1954,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1977,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -2005,7 +1996,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -2019,7 +2010,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2033,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2061,7 +2052,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2075,7 +2066,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2089,7 +2080,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2117,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2131,7 +2122,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2145,7 +2136,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2159,7 +2150,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2173,7 +2164,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2187,7 +2178,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2201,7 +2192,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2215,7 +2206,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2229,7 +2220,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2243,7 +2234,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2257,7 +2248,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2285,7 +2276,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2299,7 +2290,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2313,7 +2304,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2341,7 +2332,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2355,7 +2346,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2369,7 +2360,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2397,7 +2388,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2411,7 +2402,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2425,7 +2416,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2439,7 +2430,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2453,7 +2444,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2467,7 +2458,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2481,7 +2472,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2495,7 +2486,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2509,7 +2500,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2523,7 +2514,7 @@
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2533,11 +2524,11 @@
       <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>111</v>
+      <c r="B101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2551,7 +2542,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2565,7 +2556,7 @@
         <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2578,8 +2569,8 @@
       <c r="B104" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>53</v>
+      <c r="C104" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2589,11 +2580,11 @@
       <c r="A105" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2606,8 +2597,8 @@
       <c r="B106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>119</v>
+      <c r="C106" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2620,8 +2611,8 @@
       <c r="B107" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>31</v>
+      <c r="C107" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2635,7 +2626,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2649,7 +2640,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2663,7 +2654,7 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>17</v>
@@ -2677,7 +2668,7 @@
         <v>13</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>17</v>
@@ -2691,7 +2682,7 @@
         <v>13</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>17</v>
@@ -2705,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>17</v>
@@ -2719,7 +2710,7 @@
         <v>13</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>17</v>
@@ -2729,11 +2720,11 @@
       <c r="A115" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>126</v>
+      <c r="B115" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>17</v>
@@ -2743,72 +2734,16 @@
       <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>120</v>
+      <c r="B116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F120" s="1" t="s">
+      <c r="F116" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifica file 06_LibFormula, LIB_EWS_BE.UNION_INDICATORS, 21_Inst_Variable_BE e 22_Inst_Analysis_Unit_BE.
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="132">
   <si>
     <t>Action</t>
   </si>
@@ -433,9 +433,6 @@
   </si>
   <si>
     <t>INDICATOR_8</t>
-  </si>
-  <si>
-    <t>INDICATOR_59</t>
   </si>
   <si>
     <t>INDICATOR_62</t>
@@ -1097,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1156,7 +1153,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -1254,10 +1251,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1268,7 +1265,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1296,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1502,11 +1499,11 @@
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>110</v>
+      <c r="B28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1530,11 +1527,11 @@
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>125</v>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1562,7 +1559,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1576,7 +1573,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1589,8 +1586,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>38</v>
+      <c r="C34" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1603,8 +1600,8 @@
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>130</v>
+      <c r="C35" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1618,7 +1615,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1632,7 +1629,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1646,7 +1643,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1660,7 +1657,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1674,7 +1671,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1688,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1702,7 +1699,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1716,7 +1713,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1730,7 +1727,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1744,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1758,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1772,7 +1769,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1786,7 +1783,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1800,7 +1797,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1814,7 +1811,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1828,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1842,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1856,7 +1853,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1870,7 +1867,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1884,7 +1881,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1898,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1912,7 +1909,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1926,7 +1923,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1940,7 +1937,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1954,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1968,7 +1965,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1982,7 +1979,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1996,7 +1993,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -2010,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2024,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2038,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2052,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2066,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2080,7 +2077,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2094,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2108,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2122,7 +2119,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2136,7 +2133,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2150,7 +2147,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2164,7 +2161,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2178,7 +2175,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2192,7 +2189,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2206,7 +2203,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2220,7 +2217,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2234,7 +2231,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2248,7 +2245,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2262,7 +2259,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2276,7 +2273,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2290,7 +2287,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2304,7 +2301,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2318,7 +2315,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2332,7 +2329,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2346,7 +2343,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2360,7 +2357,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2374,7 +2371,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2388,7 +2385,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2402,7 +2399,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2416,7 +2413,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2458,7 +2455,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>17</v>
@@ -2472,7 +2469,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>17</v>
@@ -2486,7 +2483,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -2500,7 +2497,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>17</v>
@@ -2510,11 +2507,11 @@
       <c r="A100" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>52</v>
+      <c r="B100" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>17</v>
@@ -2524,11 +2521,11 @@
       <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>123</v>
+      <c r="B101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>17</v>
@@ -2542,7 +2539,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>17</v>
@@ -2555,8 +2552,8 @@
       <c r="B103" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>31</v>
+      <c r="C103" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>17</v>
@@ -2570,7 +2567,7 @@
         <v>13</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>17</v>
@@ -2584,7 +2581,7 @@
         <v>13</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>17</v>
@@ -2598,7 +2595,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>17</v>
@@ -2612,7 +2609,7 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>17</v>
@@ -2626,7 +2623,7 @@
         <v>13</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>17</v>
@@ -2640,7 +2637,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>17</v>
@@ -2654,7 +2651,7 @@
         <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>17</v>
@@ -2668,7 +2665,7 @@
         <v>13</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>17</v>
@@ -2682,7 +2679,7 @@
         <v>13</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>17</v>
@@ -2696,7 +2693,7 @@
         <v>13</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>17</v>
@@ -2706,11 +2703,11 @@
       <c r="A114" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>28</v>
+      <c r="B114" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>17</v>
@@ -2724,26 +2721,12 @@
         <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F116" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2791,12 +2774,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2914,15 +2894,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2944,16 +2934,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornamento indicatori No BIB
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="233">
   <si>
     <t>Action</t>
   </si>
@@ -469,6 +469,339 @@
   </si>
   <si>
     <t>updateAnalyticaltable_BE</t>
+  </si>
+  <si>
+    <t>INDICATOR_4</t>
+  </si>
+  <si>
+    <t>INDICATOR_5</t>
+  </si>
+  <si>
+    <t>INDICATOR_6</t>
+  </si>
+  <si>
+    <t>INDICATOR_10</t>
+  </si>
+  <si>
+    <t>INDICATOR_12</t>
+  </si>
+  <si>
+    <t>INDICATOR_17</t>
+  </si>
+  <si>
+    <t>INDICATOR_18</t>
+  </si>
+  <si>
+    <t>INDICATOR_19</t>
+  </si>
+  <si>
+    <t>INDICATOR_21</t>
+  </si>
+  <si>
+    <t>INDICATOR_22</t>
+  </si>
+  <si>
+    <t>INDICATOR_23</t>
+  </si>
+  <si>
+    <t>INDICATOR_24</t>
+  </si>
+  <si>
+    <t>INDICATOR_25</t>
+  </si>
+  <si>
+    <t>INDICATOR_26</t>
+  </si>
+  <si>
+    <t>INDICATOR_27</t>
+  </si>
+  <si>
+    <t>INDICATOR_28</t>
+  </si>
+  <si>
+    <t>INDICATOR_29</t>
+  </si>
+  <si>
+    <t>INDICATOR_30</t>
+  </si>
+  <si>
+    <t>INDICATOR_31</t>
+  </si>
+  <si>
+    <t>INDICATOR_32</t>
+  </si>
+  <si>
+    <t>INDICATOR_33</t>
+  </si>
+  <si>
+    <t>INDICATOR_36</t>
+  </si>
+  <si>
+    <t>INDICATOR_37</t>
+  </si>
+  <si>
+    <t>INDICATOR_38</t>
+  </si>
+  <si>
+    <t>INDICATOR_39</t>
+  </si>
+  <si>
+    <t>INDICATOR_41</t>
+  </si>
+  <si>
+    <t>INDICATOR_42</t>
+  </si>
+  <si>
+    <t>INDICATOR_43</t>
+  </si>
+  <si>
+    <t>INDICATOR_45</t>
+  </si>
+  <si>
+    <t>INDICATOR_46</t>
+  </si>
+  <si>
+    <t>INDICATOR_47</t>
+  </si>
+  <si>
+    <t>INDICATOR_48</t>
+  </si>
+  <si>
+    <t>INDICATOR_49</t>
+  </si>
+  <si>
+    <t>INDICATOR_50</t>
+  </si>
+  <si>
+    <t>INDICATOR_52</t>
+  </si>
+  <si>
+    <t>INDICATOR_53</t>
+  </si>
+  <si>
+    <t>INDICATOR_54</t>
+  </si>
+  <si>
+    <t>INDICATOR_57</t>
+  </si>
+  <si>
+    <t>INDICATOR_65</t>
+  </si>
+  <si>
+    <t>INDICATOR_72</t>
+  </si>
+  <si>
+    <t>INDICATOR_73</t>
+  </si>
+  <si>
+    <t>INDICATOR_90</t>
+  </si>
+  <si>
+    <t>INDICATOR_91</t>
+  </si>
+  <si>
+    <t>INDICATOR_92</t>
+  </si>
+  <si>
+    <t>INDICATOR_93</t>
+  </si>
+  <si>
+    <t>INDICATOR_99</t>
+  </si>
+  <si>
+    <t>INDICATOR_100</t>
+  </si>
+  <si>
+    <t>INDICATOR_101</t>
+  </si>
+  <si>
+    <t>INDICATOR_122</t>
+  </si>
+  <si>
+    <t>INDICATOR_123</t>
+  </si>
+  <si>
+    <t>INDICATOR_134</t>
+  </si>
+  <si>
+    <t>INDICATOR_135</t>
+  </si>
+  <si>
+    <t>INDICATOR_136</t>
+  </si>
+  <si>
+    <t>INDICATOR_137</t>
+  </si>
+  <si>
+    <t>INDICATOR_138</t>
+  </si>
+  <si>
+    <t>INDICATOR_139</t>
+  </si>
+  <si>
+    <t>INDICATOR_140</t>
+  </si>
+  <si>
+    <t>INDICATOR_141</t>
+  </si>
+  <si>
+    <t>INDICATOR_142</t>
+  </si>
+  <si>
+    <t>INDICATOR_143</t>
+  </si>
+  <si>
+    <t>INDICATOR_144</t>
+  </si>
+  <si>
+    <t>INDICATOR_145</t>
+  </si>
+  <si>
+    <t>INDICATOR_146</t>
+  </si>
+  <si>
+    <t>INDICATOR_147</t>
+  </si>
+  <si>
+    <t>INDICATOR_148</t>
+  </si>
+  <si>
+    <t>INDICATOR_149</t>
+  </si>
+  <si>
+    <t>INDICATOR_150</t>
+  </si>
+  <si>
+    <t>INDICATOR_151</t>
+  </si>
+  <si>
+    <t>INDICATOR_152</t>
+  </si>
+  <si>
+    <t>INDICATOR_153</t>
+  </si>
+  <si>
+    <t>INDICATOR_154</t>
+  </si>
+  <si>
+    <t>INDICATOR_155</t>
+  </si>
+  <si>
+    <t>INDICATOR_156</t>
+  </si>
+  <si>
+    <t>INDICATOR_157</t>
+  </si>
+  <si>
+    <t>INDICATOR_158</t>
+  </si>
+  <si>
+    <t>INDICATOR_159</t>
+  </si>
+  <si>
+    <t>INDICATOR_160</t>
+  </si>
+  <si>
+    <t>INDICATOR_161</t>
+  </si>
+  <si>
+    <t>INDICATOR_162</t>
+  </si>
+  <si>
+    <t>INDICATOR_163</t>
+  </si>
+  <si>
+    <t>INDICATOR_164</t>
+  </si>
+  <si>
+    <t>INDICATOR_165</t>
+  </si>
+  <si>
+    <t>INDICATOR_166</t>
+  </si>
+  <si>
+    <t>INDICATOR_167</t>
+  </si>
+  <si>
+    <t>INDICATOR_168</t>
+  </si>
+  <si>
+    <t>INDICATOR_169</t>
+  </si>
+  <si>
+    <t>INDICATOR_170</t>
+  </si>
+  <si>
+    <t>INDICATOR_171</t>
+  </si>
+  <si>
+    <t>INDICATOR_176</t>
+  </si>
+  <si>
+    <t>INDICATOR_177</t>
+  </si>
+  <si>
+    <t>INDICATOR_178</t>
+  </si>
+  <si>
+    <t>INDICATOR_179</t>
+  </si>
+  <si>
+    <t>INDICATOR_184</t>
+  </si>
+  <si>
+    <t>INDICATOR_185</t>
+  </si>
+  <si>
+    <t>INDICATOR_189</t>
+  </si>
+  <si>
+    <t>INDICATOR_190</t>
+  </si>
+  <si>
+    <t>INDICATOR_191</t>
+  </si>
+  <si>
+    <t>INDICATOR_192</t>
+  </si>
+  <si>
+    <t>INDICATOR_194</t>
+  </si>
+  <si>
+    <t>INDICATOR_195</t>
+  </si>
+  <si>
+    <t>INDICATOR_196</t>
+  </si>
+  <si>
+    <t>INDICATOR_198</t>
+  </si>
+  <si>
+    <t>INDICATOR_199</t>
+  </si>
+  <si>
+    <t>INDICATOR_200</t>
+  </si>
+  <si>
+    <t>INDICATOR_202</t>
+  </si>
+  <si>
+    <t>INDICATOR_203</t>
+  </si>
+  <si>
+    <t>INDICATOR_204</t>
+  </si>
+  <si>
+    <t>INDICATOR_206</t>
+  </si>
+  <si>
+    <t>INDICATOR_207</t>
+  </si>
+  <si>
+    <t>INDICATOR_208</t>
+  </si>
+  <si>
+    <t>INDICATOR_209</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C214" sqref="C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1498,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -1179,7 +1512,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -1193,7 +1526,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -1207,10 +1540,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1221,7 +1554,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -1235,7 +1568,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1249,7 +1582,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -1263,10 +1596,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1277,7 +1610,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1291,7 +1624,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>17</v>
@@ -1305,7 +1638,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1319,7 +1652,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1333,7 +1666,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -1347,7 +1680,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>17</v>
@@ -1361,7 +1694,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1375,7 +1708,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1389,7 +1722,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1403,7 +1736,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1417,7 +1750,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1431,7 +1764,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1445,7 +1778,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1459,7 +1792,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1473,7 +1806,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1487,7 +1820,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1501,7 +1834,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1515,7 +1848,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1529,7 +1862,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1543,7 +1876,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1557,7 +1890,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>56</v>
+        <v>141</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1571,7 +1904,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1585,7 +1918,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1599,7 +1932,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1613,7 +1946,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1627,7 +1960,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1641,7 +1974,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1655,7 +1988,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1669,7 +2002,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1683,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1697,7 +2030,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1711,7 +2044,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1725,7 +2058,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -1739,7 +2072,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -1753,7 +2086,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -1767,7 +2100,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1781,7 +2114,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -1795,7 +2128,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -1809,7 +2142,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -1823,7 +2156,7 @@
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -1837,7 +2170,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -1851,7 +2184,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -1865,7 +2198,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>67</v>
+        <v>158</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -1879,7 +2212,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -1893,7 +2226,7 @@
         <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -1907,7 +2240,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -1921,7 +2254,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1935,7 +2268,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -1949,7 +2282,7 @@
         <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -1963,7 +2296,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -1977,7 +2310,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -1991,7 +2324,7 @@
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2005,7 +2338,7 @@
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2019,7 +2352,7 @@
         <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2033,7 +2366,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2047,7 +2380,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2061,7 +2394,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2075,7 +2408,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2089,7 +2422,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2103,7 +2436,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2117,7 +2450,7 @@
         <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2131,7 +2464,7 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2145,7 +2478,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2159,7 +2492,7 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2173,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>17</v>
@@ -2187,7 +2520,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>17</v>
@@ -2201,7 +2534,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>17</v>
@@ -2215,7 +2548,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>17</v>
@@ -2229,7 +2562,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>17</v>
@@ -2243,7 +2576,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2257,7 +2590,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>17</v>
@@ -2271,7 +2604,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>17</v>
@@ -2285,7 +2618,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>17</v>
@@ -2299,7 +2632,7 @@
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>17</v>
@@ -2313,7 +2646,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>17</v>
@@ -2327,7 +2660,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2341,7 +2674,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>17</v>
@@ -2355,7 +2688,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>28</v>
+        <v>163</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>17</v>
@@ -2369,7 +2702,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -2383,7 +2716,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>97</v>
+        <v>165</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>17</v>
@@ -2397,7 +2730,7 @@
         <v>13</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>17</v>
@@ -2411,7 +2744,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>17</v>
@@ -2425,155 +2758,1709 @@
         <v>13</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C207" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="E207" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C208" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="E208" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C209" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" s="1" t="s">
+      <c r="E209" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C210" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="E210" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="E211" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C212" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" s="1" t="s">
+      <c r="E212" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C213" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C103" s="3" t="s">
+      <c r="E213" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C214" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="E214" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C215" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C105" s="3" t="s">
+      <c r="E215" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C106" s="3" t="s">
+      <c r="E216" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E106" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F106" s="1" t="s">
+      <c r="E217" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F217" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2589,7 +4476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2627,6 +4514,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2740,15 +4636,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
@@ -2765,6 +4652,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2778,12 +4673,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
-Aggiornamento valori di Missing -inserimento nuova formula "static_filter_indicator"
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\06_LIB_EWS_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
     <sheet name="Library_Formula" sheetId="2" r:id="rId2"/>
     <sheet name="Formula Libraries Labels" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="234">
   <si>
     <t>Action</t>
   </si>
@@ -802,6 +802,9 @@
   </si>
   <si>
     <t>INDICATOR_209</t>
+  </si>
+  <si>
+    <t>static_filter_indicators_BE</t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G217"/>
+  <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="E217" sqref="E217:F218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -4464,6 +4467,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4476,7 +4496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -4508,21 +4528,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -4636,17 +4641,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4660,17 +4681,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento gestione override BR
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/06_LIB_EWS_BE/06_LibFormula.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Library_Formula" sheetId="2" r:id="rId2"/>
     <sheet name="Formula Libraries Labels" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217:F218"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -4528,6 +4528,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -4641,22 +4656,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4670,27 +4693,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>